<commit_message>
See last commit, forgot to add -a after commit...
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
   <si>
     <t>The S-matrix contains all sample data. It is a global variable defined as a 3-dimensional matrix.</t>
   </si>
@@ -176,6 +176,45 @@
   </si>
   <si>
     <t>SSCurve</t>
+  </si>
+  <si>
+    <t>Writefield in um</t>
+  </si>
+  <si>
+    <t>Name of column dataset</t>
+  </si>
+  <si>
+    <t>GDSII database filepath</t>
+  </si>
+  <si>
+    <t>Name of structure to write</t>
+  </si>
+  <si>
+    <t>Stepszie for curves in nm</t>
+  </si>
+  <si>
+    <t>Stepsize for areas in nm</t>
+  </si>
+  <si>
+    <t>Stepsize for lines in nm</t>
+  </si>
+  <si>
+    <t>WFZoomU</t>
+  </si>
+  <si>
+    <t>WFZoomV</t>
+  </si>
+  <si>
+    <t>WFShiftU</t>
+  </si>
+  <si>
+    <t>WFShiftV</t>
+  </si>
+  <si>
+    <t>WFRotU</t>
+  </si>
+  <si>
+    <t>WFRotV</t>
   </si>
 </sst>
 </file>
@@ -530,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -880,10 +919,10 @@
         <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -894,10 +933,10 @@
         <v>49</v>
       </c>
       <c r="C36" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="D36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -908,10 +947,10 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D37" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,10 +961,10 @@
         <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>57</v>
       </c>
       <c r="D38" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -936,7 +975,7 @@
         <v>52</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>33</v>
@@ -950,7 +989,7 @@
         <v>51</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>33</v>
@@ -964,7 +1003,7 @@
         <v>53</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>17</v>
+        <v>58</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>33</v>
@@ -974,43 +1013,48 @@
       <c r="A42" s="1">
         <v>8</v>
       </c>
-      <c r="D42" t="s">
-        <v>31</v>
+      <c r="B42" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>9</v>
       </c>
-      <c r="C43" t="s">
-        <v>29</v>
-      </c>
-      <c r="D43" t="s">
-        <v>29</v>
+      <c r="B43" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>10</v>
       </c>
-      <c r="D44" t="s">
-        <v>32</v>
+      <c r="B44" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>11</v>
       </c>
-      <c r="D45" t="s">
-        <v>32</v>
+      <c r="B45" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>12</v>
       </c>
-      <c r="D46" t="s">
-        <v>31</v>
+      <c r="B46" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>13</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UNTESTED! Completed multi WF/Column settings
- Added functions:
	-> ReplaceStarbymu
	-> LastDatasettoColset

- Rewrote CollectSD and CollectUV functions
	-> Multi WF size compatible
	-> Able to save and load WF alignments
	-> Loading column settings by positionlist 'hack'

- Added possibilty to load sample data (except UV and WF coordinates) by a
  textfile called SDvars.txt
- Improved SetSvars function, able to set Column, WF and WF alignment
- Added more things todo.
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>The S-matrix contains all sample data. It is a global variable defined as a 3-dimensional matrix.</t>
   </si>
@@ -103,9 +103,6 @@
     <t>GDSII</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Layers to expose (; separated)</t>
   </si>
   <si>
@@ -139,9 +136,6 @@
     <t>Layer 61 switch</t>
   </si>
   <si>
-    <t>Full GDSII datapath</t>
-  </si>
-  <si>
     <t>WF</t>
   </si>
   <si>
@@ -215,6 +209,24 @@
   </si>
   <si>
     <t>WFRotV</t>
+  </si>
+  <si>
+    <t>n-Samples</t>
+  </si>
+  <si>
+    <t>Number of samples</t>
+  </si>
+  <si>
+    <t>Procedure</t>
+  </si>
+  <si>
+    <t>Procedure of var collecting</t>
+  </si>
+  <si>
+    <t>1 = One dataset for all samples, 2 = Use separate dataset per sample</t>
+  </si>
+  <si>
+    <t>1 = Use only photomarkers, 2 = Use both photo and EBL markers, 3 = Only do one WF alignment on the first device on a chip, 4 = Do no WF alignment at all</t>
   </si>
 </sst>
 </file>
@@ -569,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +593,7 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,7 +603,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,7 +631,7 @@
         <v>10</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -632,7 +645,7 @@
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -646,7 +659,7 @@
         <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -660,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="D9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -674,7 +687,7 @@
         <v>14</v>
       </c>
       <c r="D10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -688,7 +701,7 @@
         <v>15</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -702,15 +715,15 @@
         <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -724,7 +737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -732,13 +745,13 @@
         <v>18</v>
       </c>
       <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -746,13 +759,13 @@
         <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -760,13 +773,13 @@
         <v>21</v>
       </c>
       <c r="C20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -774,13 +787,13 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -788,13 +801,13 @@
         <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -802,13 +815,13 @@
         <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D23" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -816,13 +829,13 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D24" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -830,27 +843,30 @@
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D25" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>9</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="D26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>10</v>
       </c>
@@ -858,43 +874,43 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="C28" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -916,13 +932,13 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -930,13 +946,13 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D36" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -947,10 +963,10 @@
         <v>28</v>
       </c>
       <c r="C37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -958,13 +974,13 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -972,13 +988,13 @@
         <v>5</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -986,13 +1002,13 @@
         <v>6</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1000,13 +1016,13 @@
         <v>7</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,7 +1030,7 @@
         <v>8</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1022,7 +1038,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1030,7 +1046,7 @@
         <v>10</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1038,7 +1054,7 @@
         <v>11</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1046,7 +1062,7 @@
         <v>12</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1054,10 +1070,11 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Small incremental fix of a bracket.
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Loading WF markers + procedures from files
(Needs some testing)
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="S-Matrix" sheetId="1" r:id="rId1"/>
+    <sheet name="Markertypes" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="110">
   <si>
     <t>The S-matrix contains all sample data. It is a global variable defined as a 3-dimensional matrix.</t>
   </si>
@@ -254,6 +255,96 @@
   </si>
   <si>
     <t>Beamcurrent in nA</t>
+  </si>
+  <si>
+    <t>Markertype[q]</t>
+  </si>
+  <si>
+    <t>Markername</t>
+  </si>
+  <si>
+    <t>Upos</t>
+  </si>
+  <si>
+    <t>Vpos</t>
+  </si>
+  <si>
+    <t>SizeU</t>
+  </si>
+  <si>
+    <t>SizeV</t>
+  </si>
+  <si>
+    <t>StepU</t>
+  </si>
+  <si>
+    <t>StepV</t>
+  </si>
+  <si>
+    <t>PointsV</t>
+  </si>
+  <si>
+    <t>PointsU</t>
+  </si>
+  <si>
+    <t>MarkOffsetU</t>
+  </si>
+  <si>
+    <t>MarkOffsetV</t>
+  </si>
+  <si>
+    <t>MarkplaceU</t>
+  </si>
+  <si>
+    <t>MarkplaceV</t>
+  </si>
+  <si>
+    <t>Profile min</t>
+  </si>
+  <si>
+    <t>Profile max</t>
+  </si>
+  <si>
+    <t>ContrastLow</t>
+  </si>
+  <si>
+    <t>ContrastHigh</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>Entry positionlist</t>
+  </si>
+  <si>
+    <t>Entry</t>
+  </si>
+  <si>
+    <t>WFAlignprocedures[q]</t>
+  </si>
+  <si>
+    <t>..</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>last</t>
+  </si>
+  <si>
+    <t>Procedurename</t>
+  </si>
+  <si>
+    <t>entries (inc. log)</t>
+  </si>
+  <si>
+    <t>1st entry</t>
+  </si>
+  <si>
+    <t>2nd entry</t>
+  </si>
+  <si>
+    <t>etc</t>
   </si>
 </sst>
 </file>
@@ -289,7 +380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -298,6 +389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,7 +696,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
@@ -1190,4 +1282,225 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="E6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>87</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+      <c r="E8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ability to specify number of exposureloops, automatically adjusting the base dose for the correct total exposure
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="-31360" yWindow="-11520" windowWidth="28940" windowHeight="18860"/>
   </bookViews>
   <sheets>
     <sheet name="S-Matrix" sheetId="1" r:id="rId1"/>
     <sheet name="Markertypes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="122211" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="115">
   <si>
     <t>The S-matrix contains all sample data. It is a global variable defined as a 3-dimensional matrix.</t>
   </si>
@@ -351,18 +356,34 @@
   </si>
   <si>
     <t>WFMethod</t>
+  </si>
+  <si>
+    <t>Three-point UV alignment settings</t>
+  </si>
+  <si>
+    <t>ExposureLoops</t>
+  </si>
+  <si>
+    <t>Number of exposure loops</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -386,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -396,6 +417,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,7 +478,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -491,7 +513,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,30 +724,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="1"/>
+    <col min="2" max="2" width="19.1640625" customWidth="1"/>
+    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="67.85546875" customWidth="1"/>
+    <col min="5" max="5" width="67.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="B4" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -739,7 +764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -753,7 +778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -767,7 +792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -781,7 +806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -795,7 +820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -809,7 +834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -823,7 +848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -837,12 +862,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="B16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -856,7 +881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -870,7 +895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -884,7 +909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -898,7 +923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -912,7 +937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -926,7 +951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -940,7 +965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -954,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -968,7 +993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>9</v>
       </c>
@@ -985,7 +1010,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>10</v>
       </c>
@@ -1002,7 +1027,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>11</v>
       </c>
@@ -1016,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>12</v>
       </c>
@@ -1030,7 +1055,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>13</v>
       </c>
@@ -1044,7 +1069,21 @@
         <v>110</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5">
+      <c r="A31" s="1">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" t="s">
+        <v>114</v>
+      </c>
+      <c r="D31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1058,7 +1097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1072,7 +1111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1086,7 +1125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -1100,7 +1139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -1114,7 +1153,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>5</v>
       </c>
@@ -1128,7 +1167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>6</v>
       </c>
@@ -1142,7 +1181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>7</v>
       </c>
@@ -1156,7 +1195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -1170,7 +1209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>9</v>
       </c>
@@ -1184,7 +1223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>10</v>
       </c>
@@ -1198,12 +1237,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4">
       <c r="B47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -1217,7 +1256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4">
       <c r="A49" s="3">
         <v>2</v>
       </c>
@@ -1231,7 +1270,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -1245,7 +1284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4">
       <c r="A51" s="3">
         <v>4</v>
       </c>
@@ -1259,7 +1298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4">
       <c r="A52" s="3">
         <v>5</v>
       </c>
@@ -1273,7 +1312,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4">
       <c r="A53" s="3">
         <v>6</v>
       </c>
@@ -1287,7 +1326,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4">
       <c r="A54" s="3">
         <v>7</v>
       </c>
@@ -1303,7 +1342,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1315,13 +1359,13 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>79</v>
       </c>
@@ -1332,7 +1376,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1346,7 +1390,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1360,7 +1404,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1374,7 +1418,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1388,7 +1432,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1402,7 +1446,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1413,7 +1457,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1427,7 +1471,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1435,7 +1479,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1443,7 +1487,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1451,7 +1495,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1459,7 +1503,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1467,7 +1511,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1475,7 +1519,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1483,7 +1527,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1491,7 +1535,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1499,7 +1543,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1507,7 +1551,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1515,7 +1559,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1525,5 +1569,10 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed bug where beamcurrent was not collected properly when using
single-settings mode. This resulted in a 'beam current out of bounds'
error message and further patterning was interrupted.
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="25306"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-31360" yWindow="-11520" windowWidth="28940" windowHeight="18860"/>
+    <workbookView xWindow="-31365" yWindow="-11520" windowWidth="28935" windowHeight="18855"/>
   </bookViews>
   <sheets>
     <sheet name="S-Matrix" sheetId="1" r:id="rId1"/>
@@ -250,9 +250,6 @@
     <t>Beamspeed for lines in mm/s</t>
   </si>
   <si>
-    <t>Beamspeed for curvse in mm/s</t>
-  </si>
-  <si>
     <t>BeamCurrent</t>
   </si>
   <si>
@@ -365,6 +362,9 @@
   </si>
   <si>
     <t>Number of exposure loops</t>
+  </si>
+  <si>
+    <t>Beamspeed for curves in mm/s</t>
   </si>
 </sst>
 </file>
@@ -724,33 +724,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="19.1640625" customWidth="1"/>
-    <col min="3" max="3" width="37.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
-    <col min="5" max="5" width="67.83203125" customWidth="1"/>
+    <col min="5" max="5" width="67.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -764,7 +764,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -778,7 +778,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -792,7 +792,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -806,7 +806,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -820,7 +820,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -834,7 +834,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -848,7 +848,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -862,12 +862,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
@@ -881,7 +881,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>1</v>
       </c>
@@ -895,7 +895,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>2</v>
       </c>
@@ -909,7 +909,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>3</v>
       </c>
@@ -923,7 +923,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>4</v>
       </c>
@@ -937,7 +937,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>5</v>
       </c>
@@ -951,7 +951,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>6</v>
       </c>
@@ -965,7 +965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>7</v>
       </c>
@@ -979,7 +979,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>8</v>
       </c>
@@ -993,7 +993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>9</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>10</v>
       </c>
@@ -1024,10 +1024,10 @@
         <v>30</v>
       </c>
       <c r="E27" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>11</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>12</v>
       </c>
@@ -1055,35 +1055,35 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D30" t="s">
         <v>31</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>14</v>
       </c>
       <c r="B31" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" t="s">
         <v>113</v>
-      </c>
-      <c r="C31" t="s">
-        <v>114</v>
       </c>
       <c r="D31" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>1</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -1153,7 +1153,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>5</v>
       </c>
@@ -1167,7 +1167,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>6</v>
       </c>
@@ -1181,7 +1181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>7</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -1209,7 +1209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>9</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>10</v>
       </c>
@@ -1237,12 +1237,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>1</v>
       </c>
@@ -1256,7 +1256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>2</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>3</v>
       </c>
@@ -1284,7 +1284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>4</v>
       </c>
@@ -1298,7 +1298,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>5</v>
       </c>
@@ -1312,7 +1312,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>6</v>
       </c>
@@ -1320,21 +1320,21 @@
         <v>73</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>7</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C54" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D54" s="2" t="s">
         <v>32</v>
@@ -1359,212 +1359,212 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Major update, grab UV+WF function, loooooots of input checks everywhere
-Input checks for loading .txt files
-Input checks for collecting data in script
-Variable types are now handled properly
-Cancel now aborts script as intended
-Logs everything if script is cancelled during data collection
-Marker entries in Alignprocedures.txt are now cross checked with markers
in Markers.txt on startup
-RAITH User is added to the title of the log (and as a log entry)
-Renamed GDSmarkers.txt to L61markers.txt
-Added option to only do a L61 alignment on the 1st structure of a sample
-A few more panicbutton checks
-Numerous small rewrites
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-31365" yWindow="-11520" windowWidth="28935" windowHeight="18855"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="117">
-  <si>
-    <t>The S-matrix contains all sample data. It is a global variable defined as a 3-dimensional matrix.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="119">
   <si>
     <t>[x]</t>
   </si>
@@ -136,9 +133,6 @@
     <t>Procedure defined in WFAutoAlign</t>
   </si>
   <si>
-    <t>Layer 61 switch</t>
-  </si>
-  <si>
     <t>WF</t>
   </si>
   <si>
@@ -371,6 +365,18 @@
   </si>
   <si>
     <t>% overpattern used</t>
+  </si>
+  <si>
+    <t>Layer 61 string</t>
+  </si>
+  <si>
+    <t>-1 if L61 is not used, marker-procedure-layers when used.</t>
+  </si>
+  <si>
+    <t>The S-matrix contains all sample data. It is a 3-dimensional array defined as a global variable.</t>
+  </si>
+  <si>
+    <t>For [y] = 5 and [z] = i</t>
   </si>
 </sst>
 </file>
@@ -517,6 +523,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -552,6 +575,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -730,14 +770,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" customWidth="1"/>
     <col min="5" max="5" width="67.85546875" customWidth="1"/>
@@ -745,29 +785,29 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -775,13 +815,13 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,13 +829,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -803,13 +843,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,13 +857,13 @@
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,13 +871,13 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,13 +885,13 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,32 +899,32 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
       <c r="D12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" t="s">
-        <v>9</v>
-      </c>
       <c r="D17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -892,13 +932,13 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" t="s">
         <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -906,13 +946,13 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -920,13 +960,13 @@
         <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -934,13 +974,13 @@
         <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -948,13 +988,13 @@
         <v>5</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -962,13 +1002,13 @@
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -976,13 +1016,13 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -990,13 +1030,13 @@
         <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1004,16 +1044,16 @@
         <v>9</v>
       </c>
       <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>65</v>
+      </c>
+      <c r="D26" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" t="s">
         <v>66</v>
-      </c>
-      <c r="C26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,16 +1061,16 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,13 +1078,13 @@
         <v>11</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1052,13 +1092,16 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>38</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1066,13 +1109,13 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E30" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,27 +1123,32 @@
         <v>14</v>
       </c>
       <c r="B31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
+        <v>7</v>
+      </c>
+      <c r="C34" t="s">
         <v>8</v>
       </c>
-      <c r="C34" t="s">
-        <v>9</v>
-      </c>
       <c r="D34" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1108,13 +1156,13 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1122,13 +1170,13 @@
         <v>2</v>
       </c>
       <c r="B36" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C36" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1136,13 +1184,13 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,13 +1198,13 @@
         <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C38" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1164,13 +1212,13 @@
         <v>5</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,13 +1226,13 @@
         <v>6</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,13 +1240,13 @@
         <v>7</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,13 +1254,13 @@
         <v>8</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,13 +1268,13 @@
         <v>9</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1234,18 +1282,18 @@
         <v>10</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,13 +1301,13 @@
         <v>1</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1267,13 +1315,13 @@
         <v>2</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1281,13 +1329,13 @@
         <v>3</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,13 +1343,13 @@
         <v>4</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1309,13 +1357,13 @@
         <v>5</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="D52" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1323,13 +1371,13 @@
         <v>6</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1337,13 +1385,13 @@
         <v>7</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1351,13 +1399,13 @@
         <v>8</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1387,13 +1435,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1401,13 +1449,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1415,13 +1463,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1429,13 +1477,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D4">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1443,13 +1491,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D5">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1457,13 +1505,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1471,10 +1519,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1482,13 +1530,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1496,7 +1544,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1504,7 +1552,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,7 +1560,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1520,7 +1568,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1528,7 +1576,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1536,7 +1584,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1544,7 +1592,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,7 +1600,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1560,7 +1608,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1568,7 +1616,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1576,7 +1624,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1584,7 +1632,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added check for column dataset, added WorkingArea to sample parameters,
 fixed beamcurrent measurement bug, started a manual.
</commit_message>
<xml_diff>
--- a/S-matrix_doc.xlsx
+++ b/S-matrix_doc.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-31365" yWindow="-11520" windowWidth="28935" windowHeight="18855"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="122">
   <si>
     <t>[x]</t>
   </si>
@@ -377,6 +377,15 @@
   </si>
   <si>
     <t>For [y] = 5 and [z] = i</t>
+  </si>
+  <si>
+    <t>WorkingArea</t>
+  </si>
+  <si>
+    <t>Edges of working area (um)</t>
+  </si>
+  <si>
+    <t>bottomleft U, bottomleft V, upperright U, upperright V</t>
   </si>
 </sst>
 </file>
@@ -770,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="115" zoomScaleNormal="115" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1132,12 +1141,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1160,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>1</v>
       </c>
@@ -1165,7 +1174,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>2</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>3</v>
       </c>
@@ -1193,7 +1202,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>4</v>
       </c>
@@ -1207,7 +1216,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>5</v>
       </c>
@@ -1221,7 +1230,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>6</v>
       </c>
@@ -1235,7 +1244,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>7</v>
       </c>
@@ -1249,7 +1258,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>8</v>
       </c>
@@ -1263,7 +1272,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>9</v>
       </c>
@@ -1277,7 +1286,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>10</v>
       </c>
@@ -1291,12 +1300,29 @@
         <v>31</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>11</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>1</v>
       </c>

</xml_diff>